<commit_message>
Update Docker [Elasticsearch + SSH] + Documentation
</commit_message>
<xml_diff>
--- a/AWS/Test_ELKs.xlsx
+++ b/AWS/Test_ELKs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="135" windowWidth="22110" windowHeight="8760"/>
+    <workbookView xWindow="285" yWindow="135" windowWidth="20730" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,9 +544,9 @@
     <col min="2" max="2" width="11.5703125" style="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1060,13 +1060,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2"/>
-    <hyperlink ref="J3"/>
-    <hyperlink ref="J4"/>
-    <hyperlink ref="J5"/>
-    <hyperlink ref="J13"/>
-    <hyperlink ref="J15"/>
-    <hyperlink ref="J14"/>
+    <hyperlink ref="J2" display="https://search-elkservicearchitecture-jz4sluz2voumevqhnh4gdntkgm.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover?_a=(columns:!(_source),index:'logstash-*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'*')),sort:!('@timestamp',desc))&amp;_"/>
+    <hyperlink ref="J3" display="https://search-elkservicearchitecture-jz4sluz2voumevqhnh4gdntkgm.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover?_a=(columns:!(_source),index:'logstash-*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'*')),sort:!('@timestamp',desc))&amp;_"/>
+    <hyperlink ref="J4" display="https://search-elkservicearchitecture-jz4sluz2voumevqhnh4gdntkgm.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-05-26T09:30:51.624Z',mode:absolute,to:'2016-05-26T09:41:16.721Z'))&amp;_"/>
+    <hyperlink ref="J5" display="https://search-elkservicearchitecture-jz4sluz2voumevqhnh4gdntkgm.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover?_a=(columns:!(_source),index:'logstash-*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'*')),sort:!('@timestamp',desc))&amp;_"/>
+    <hyperlink ref="J13" display="http://ec2-52-203-178-151.compute-1.amazonaws.com:5601/app/kibana#/discover?_g=(refreshInterval:(display:Off,pause:!f,value:0),time:(from:'2016-05-26T10:47:56.035Z',mode:absolute,to:'2016-05-26T10:49:24.960Z'))&amp;_a=(columns:!(_source),index:'logstash-*',in"/>
+    <hyperlink ref="J15" display="http://ec2-52-203-178-151.compute-1.amazonaws.com:5601/app/kibana#/discover?_g=(refreshInterval:(display:Off,pause:!f,value:0),time:(from:'2016-05-26T11:07:39.714Z',mode:absolute,to:'2016-05-26T11:16:23.907Z'))&amp;_a=(columns:!(_source),index:'logstash-*',in"/>
+    <hyperlink ref="J14" display="http://ec2-52-203-178-151.compute-1.amazonaws.com:5601/app/kibana#/discover?_g=(refreshInterval:(display:Off,pause:!f,value:0),time:(from:'2016-05-26T10:55:44.920Z',mode:absolute,to:'2016-05-26T10:58:00.000Z'))&amp;_a=(columns:!(_source),index:'logstash-*',in"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>